<commit_message>
My first Web Scrapping program Code
</commit_message>
<xml_diff>
--- a/iMDB Movie Rating.xlsx
+++ b/iMDB Movie Rating.xlsx
@@ -4125,12 +4125,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>The Bridge on the River Kwai</t>
+          <t>Trainspotting</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>1996</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -4147,12 +4147,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Trainspotting</t>
+          <t>The Bridge on the River Kwai</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">

</xml_diff>